<commit_message>
updated eHistory.07 suggested list
</commit_message>
<xml_diff>
--- a/SuggestedLists/eHistory.07 - Environmental Food Allergies.xlsx
+++ b/SuggestedLists/eHistory.07 - Environmental Food Allergies.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="189">
   <si>
     <t>SNOMED CT Code</t>
   </si>
@@ -575,6 +575,12 @@
   </si>
   <si>
     <t>Sunlight (skin sensitivity to sun)</t>
+  </si>
+  <si>
+    <t>Feather</t>
+  </si>
+  <si>
+    <t>NEMSIS TAC Update 11-08-2016</t>
   </si>
 </sst>
 </file>
@@ -654,7 +660,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -699,6 +705,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -969,7 +976,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -977,11 +984,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I103"/>
+  <dimension ref="A1:I104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1001,1065 +1008,1076 @@
       <c r="C1" s="12"/>
       <c r="D1" s="13"/>
     </row>
-    <row r="2" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="13"/>
+    </row>
+    <row r="3" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B3" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="2"/>
-    </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="9">
-        <v>403141006</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
-        <v>84</v>
+        <v>4</v>
       </c>
       <c r="C6" s="9">
-        <v>424213003</v>
+        <v>403141006</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C7" s="9">
-        <v>232346004</v>
+        <v>424213003</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="C8" s="9">
-        <v>15911003</v>
+        <v>232346004</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="C9" s="9">
-        <v>232347008</v>
+        <v>15911003</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C10" s="9">
+        <v>232347008</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C11" s="9">
         <v>419271008</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="9">
-        <v>232348003</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
-        <v>37</v>
+        <v>187</v>
       </c>
       <c r="C12" s="9">
-        <v>307427009</v>
+        <v>232348003</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="C13" s="9">
-        <v>419063004</v>
+        <v>307427009</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C14" s="9">
-        <v>422921000</v>
+        <v>419063004</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C15" s="9">
-        <v>427487000</v>
+        <v>422921000</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="9">
+        <v>427487000</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C17" s="9">
         <v>423058007</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D17" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="D17" s="13"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C18" s="9">
-        <v>106190000</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>50</v>
-      </c>
+      <c r="D18" s="13"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
-        <v>47</v>
+        <v>150</v>
       </c>
       <c r="C19" s="9">
-        <v>160244002</v>
+        <v>106190000</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="9">
+        <v>160244002</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C21" s="9">
         <v>444316004</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="D21" s="13"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C22" s="9">
-        <v>390952000</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="D22" s="13"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="C23" s="9">
-        <v>426232007</v>
+        <v>390952000</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C24" s="9">
-        <v>418689008</v>
+        <v>426232007</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C25" s="9">
-        <v>419474003</v>
+        <v>418689008</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C26" s="9">
-        <v>294619002</v>
+        <v>419474003</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
-        <v>151</v>
+        <v>99</v>
       </c>
       <c r="C27" s="9">
-        <v>402594000</v>
+        <v>294619002</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
-        <v>98</v>
+        <v>151</v>
       </c>
       <c r="C28" s="9">
-        <v>300910009</v>
+        <v>402594000</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">
-        <v>172</v>
+        <v>98</v>
       </c>
       <c r="C29" s="9">
-        <v>419101002</v>
+        <v>300910009</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="C30" s="9">
-        <v>258155009</v>
+        <v>419101002</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="7" t="s">
-        <v>122</v>
+        <v>186</v>
       </c>
       <c r="C31" s="9">
-        <v>402595004</v>
+        <v>258155009</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C32" s="9">
+        <v>402595004</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C33" s="9">
         <v>425605001</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D33" s="6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="D33" s="18"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C34" s="19">
-        <v>409136006</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="D34" s="18"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C35" s="19">
-        <v>419342009</v>
+        <v>409136006</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C36" s="19">
+        <v>419342009</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C36" s="19">
+      <c r="C37" s="19">
         <v>420174000</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D37" s="6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="13"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C38" s="19">
-        <v>420080006</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>9</v>
-      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="13"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C39" s="19">
-        <v>419573007</v>
+        <v>420080006</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C40" s="19">
-        <v>91932007</v>
+        <v>419573007</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B41" s="3" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="C41" s="19">
-        <v>294316000</v>
+        <v>91932007</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
-        <v>140</v>
+        <v>104</v>
       </c>
       <c r="C42" s="19">
-        <v>91938006</v>
+        <v>294316000</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C43" s="19">
+        <v>91938006</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C43" s="19">
+      <c r="C44" s="19">
         <v>418779002</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D44" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D44" s="18"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C45" s="9">
-        <v>712839001</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>181</v>
-      </c>
+      <c r="D45" s="18"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C46" s="10">
-        <v>712838009</v>
+        <v>175</v>
+      </c>
+      <c r="C46" s="9">
+        <v>712839001</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C47" s="19">
-        <v>419814004</v>
+        <v>174</v>
+      </c>
+      <c r="C47" s="10">
+        <v>712838009</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I47" s="7"/>
+        <v>183</v>
+      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C48" s="19">
+        <v>419814004</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I48" s="7"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="C48" s="10">
+      <c r="C49" s="10">
         <v>712840004</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D49" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="49" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="3" t="s">
+    <row r="50" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C49" s="9">
+      <c r="C50" s="9">
         <v>91934008</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D50" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="I49" s="1"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="C50" s="19">
-        <v>91935009</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="I50" s="1"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C51" s="19">
+        <v>91935009</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="C51" s="19">
+      <c r="C52" s="19">
         <v>91940001</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D52" s="5" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="7" t="s">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="D52" s="18"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B53" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C53" s="19">
-        <v>417532002</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>28</v>
-      </c>
+      <c r="D53" s="18"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
       <c r="C54" s="19">
-        <v>300913006</v>
+        <v>417532002</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C55" s="19">
+        <v>300913006</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C55" s="19">
+      <c r="C56" s="19">
         <v>419972009</v>
       </c>
-      <c r="D55" s="6" t="s">
+      <c r="D56" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="D56" s="18"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B57" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C57" s="19">
-        <v>300914000</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="D57" s="18"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C58" s="19">
-        <v>300912001</v>
+        <v>300914000</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="C59" s="19">
-        <v>418397007</v>
+        <v>300912001</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C60" s="19">
-        <v>425525006</v>
+        <v>418397007</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C61" s="19">
-        <v>91930004</v>
+        <v>425525006</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
-        <v>88</v>
+        <v>129</v>
       </c>
       <c r="C62" s="19">
-        <v>414285001</v>
+        <v>91930004</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="C63" s="19">
-        <v>294847001</v>
+        <v>414285001</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
-        <v>33</v>
+        <v>103</v>
       </c>
       <c r="C64" s="19">
-        <v>441831003</v>
+        <v>294847001</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
-        <v>89</v>
+        <v>33</v>
       </c>
       <c r="C65" s="19">
-        <v>447961002</v>
+        <v>441831003</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
-        <v>157</v>
+        <v>89</v>
       </c>
       <c r="C66" s="19">
-        <v>419619007</v>
+        <v>447961002</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="C67" s="19">
-        <v>25868003</v>
+        <v>419619007</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C68" s="19">
+        <v>25868003</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C68" s="19">
+      <c r="C69" s="19">
         <v>419421008</v>
       </c>
-      <c r="D68" s="6" t="s">
+      <c r="D69" s="6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="D69" s="18"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C70" s="19">
-        <v>417918006</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>58</v>
-      </c>
+      <c r="D70" s="18"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C71" s="19">
+        <v>417918006</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C71" s="19">
+      <c r="C72" s="19">
         <v>418815008</v>
       </c>
-      <c r="D71" s="6" t="s">
+      <c r="D72" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="7" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="D72" s="13"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="C73" s="9">
-        <v>294420000</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>1</v>
-      </c>
+      <c r="D73" s="13"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B74" s="7" t="s">
-        <v>144</v>
+        <v>107</v>
       </c>
       <c r="C74" s="9">
-        <v>419180003</v>
+        <v>294420000</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B75" s="7" t="s">
-        <v>108</v>
+        <v>144</v>
       </c>
       <c r="C75" s="9">
-        <v>294434000</v>
+        <v>419180003</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B76" s="7" t="s">
-        <v>145</v>
+        <v>108</v>
       </c>
       <c r="C76" s="9">
-        <v>418344001</v>
+        <v>294434000</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B77" s="7" t="s">
-        <v>100</v>
+        <v>145</v>
       </c>
       <c r="C77" s="9">
-        <v>294318004</v>
+        <v>418344001</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B78" s="7" t="s">
-        <v>147</v>
+        <v>100</v>
       </c>
       <c r="C78" s="9">
-        <v>418545001</v>
+        <v>294318004</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B79" s="7" t="s">
-        <v>110</v>
+        <v>147</v>
       </c>
       <c r="C79" s="9">
-        <v>294298002</v>
+        <v>418545001</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B80" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C80" s="9">
-        <v>293817009</v>
+        <v>294298002</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B81" s="7" t="s">
-        <v>160</v>
+        <v>112</v>
       </c>
       <c r="C81" s="9">
-        <v>294321002</v>
+        <v>293817009</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B82" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C82" s="9">
+        <v>294321002</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B83" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C82" s="9">
+      <c r="C83" s="9">
         <v>300908007</v>
       </c>
-      <c r="D82" s="6" t="s">
+      <c r="D83" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B83" s="3" t="s">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B84" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C83" s="9">
+      <c r="C84" s="9">
         <v>293842000</v>
       </c>
-      <c r="D83" s="6" t="s">
+      <c r="D84" s="6" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B84" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="C84" s="9">
-        <v>294923007</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B85" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C85" s="9">
-        <v>294924001</v>
+        <v>294923007</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B86" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C86" s="9">
+        <v>294924001</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B87" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="C86" s="9">
+      <c r="C87" s="9">
         <v>294925000</v>
       </c>
-      <c r="D86" s="6" t="s">
+      <c r="D87" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="7" t="s">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="D87" s="13"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B88" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C88" s="9">
-        <v>294169006</v>
-      </c>
-      <c r="D88" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="D88" s="13"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B89" s="7" t="s">
-        <v>146</v>
+        <v>109</v>
       </c>
       <c r="C89" s="9">
-        <v>417982003</v>
+        <v>294169006</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B90" s="7" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="C90" s="9">
-        <v>418968001</v>
+        <v>417982003</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B91" s="7" t="s">
-        <v>111</v>
+        <v>159</v>
       </c>
       <c r="C91" s="9">
-        <v>300916003</v>
+        <v>418968001</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B92" s="7" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C92" s="9">
-        <v>294324005</v>
+        <v>300916003</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B93" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C93" s="9">
+        <v>294324005</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B94" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C93" s="9">
+      <c r="C94" s="9">
         <v>419412007</v>
       </c>
-      <c r="D93" s="6" t="s">
+      <c r="D94" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="94" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="7" t="s">
+    <row r="95" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="C94" s="9">
+      <c r="C95" s="9">
         <v>294328008</v>
       </c>
-      <c r="D94" s="6" t="s">
+      <c r="D95" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="I94" s="1"/>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B95" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C95" s="9">
-        <v>419199007</v>
-      </c>
-      <c r="D95" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="I95" s="1"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B96" s="7" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="C96" s="9">
-        <v>294179008</v>
+        <v>419199007</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>72</v>
+        <v>13</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B97" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C97" s="9">
+        <v>294179008</v>
+      </c>
+      <c r="D97" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B98" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="C97" s="9">
+      <c r="C98" s="9">
         <v>405649006</v>
       </c>
-      <c r="D97" s="6" t="s">
+      <c r="D98" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="I97" s="7"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A98" s="7" t="s">
+      <c r="I98" s="7"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="D98" s="13"/>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B99" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="C99" s="9">
-        <v>402306009</v>
-      </c>
-      <c r="D99" s="6" t="s">
-        <v>2</v>
-      </c>
+      <c r="D99" s="13"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B100" s="7" t="s">
-        <v>119</v>
+        <v>148</v>
       </c>
       <c r="C100" s="9">
-        <v>294238000</v>
+        <v>402306009</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B101" s="7" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="C101" s="9">
-        <v>300915004</v>
+        <v>294238000</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B102" s="7" t="s">
-        <v>149</v>
+        <v>91</v>
       </c>
       <c r="C102" s="9">
-        <v>419788000</v>
+        <v>300915004</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B103" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C103" s="9">
+        <v>419788000</v>
+      </c>
+      <c r="D103" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B104" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C103" s="9">
+      <c r="C104" s="9">
         <v>294950002</v>
       </c>
-      <c r="D103" s="6" t="s">
+      <c r="D104" s="6" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>